<commit_message>
Save before board restructuring
</commit_message>
<xml_diff>
--- a/Error Testing 1.xlsx
+++ b/Error Testing 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myerauedu-my.sharepoint.com/personal/bramhalc_my_erau_edu/Documents/School 2020 Fall/EGR 115/ManyPlayerChess/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_18B4994B0EAE5FD075CF3DD85D9A4843AA16CD01" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C302E6AD-AC1B-4840-92F4-9F3B5E2B09DE}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_18B4994B0EAE5FD075CF3DD85D9A4843AA16CD01" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADA8B868-8A10-4292-BA9F-27D098F0195F}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="2436" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -349,8 +349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -360,7 +360,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>9</v>
@@ -369,7 +369,7 @@
         <v>0</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>